<commit_message>
add update comentários iniciais de cada bloco de scripts por revisão
</commit_message>
<xml_diff>
--- a/resultado_consulta_cnae_I.xlsx
+++ b/resultado_consulta_cnae_I.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:I181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7060,6 +7060,1886 @@
         </is>
       </c>
     </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>01.764.052/0001-05</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>SUPERMERCADO DEZ DE ABRIL LTDA</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Açu</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>redeidealdezabril@yahoo.com.br</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01764052000105</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>4711-3/02</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>Comércio varejista de mercadorias em geral, com predominância de produtos alimentícios - supermercados</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:34:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>01.764.234/0001-78</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>MAGI CLEAN ADMINISTRACAO DE SERVICOS LTDA</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>AM</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Manaus</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>não cadastrado</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01764234000178</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>8121-4/00</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Limpeza em prédios e em domicílios</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:34:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>01.764.237/0001-01</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>TRANSPORTES DIJEPE LTDA</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Ibirubá</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>pedrotti_11@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01764237000101</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>4930-2/02</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Transporte rodoviário de carga, exceto produtos perigosos e mudanças, intermunicipal, interestadual e internacional</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:35:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>01.764.411/0001-16</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>TV CIDADE DOS PRINCIPES LTDA</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Joinville</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>contabilidade@ndtv.com.br</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01764411000116</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>6021-7/00</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Atividades de televisão aberta</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:35:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>01.764.417/0001-93</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>METRA-SISTEMA METROPOLITANO DE TRANSPORTES LTDA</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>São Bernardo do Campo</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>dr@metra.com.br</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01764417000193</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>4921-3/02</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Transporte rodoviário coletivo de passageiros, com itinerário fixo, intermunicipal em região metropolitana</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:35:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>01.764.484/0001-08</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>RESTAURANTE AOYAMAS LTDA</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>dorian@restauranteaoyama.com.br</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01764484000108</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>5611-2/01</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Restaurantes e similares</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:36:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>01.764.496/0001-32</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>BEI COMUNICACAO LTDA</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>raquel.panhan@bei.com.br</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01764496000132</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>5811-5/00</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Edição de livros</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:36:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>01.764.578/0001-87</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>ALOISIO BRITO DE SANTANA</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Camamu</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>administrativo@dreamcont.com.br</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01764578000187</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>4731-8/00</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>Comércio varejista de combustíveis para veículos automotores</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:37:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>01.764.629/0001-70</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>MERSALUC COMERCIAL DE ALIMENTOS LTDA</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Teixeira de Freitas</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>mersaluc@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01764629000170</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>4711-3/02</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>Comércio varejista de mercadorias em geral, com predominância de produtos alimentícios - supermercados</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:37:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>01.764.685/0001-05</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>ANTONIO &amp; BARBOSA LTDA</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Jequitinhonha</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>siare@escritaonline.cnt.br</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01764685000105</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>4712-1/00</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>Comércio varejista de mercadorias em geral, com predominância de produtos alimentícios - minimercados, mercearias e armazéns</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:37:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>01.765.080/0001-39</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>AUTO POSTO BOMTEMPO LTDA</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Nova Xavantina</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>andreaftb@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01765080000139</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>4731-8/00</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>Comércio varejista de combustíveis para veículos automotores</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:38:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>01.765.151/0001-01</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>FLUITEK COMPONENTES DE PROCESSO LTDA</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Campinas</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>andre@fluitek.com.br</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01765151000101</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>4663-0/00</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>Comércio atacadista de máquinas e equipamentos para uso industrial; partes e peças</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:38:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>01.765.332/0001-20</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>BEZERRA COMERCIO DE COMBUSTIVEIS LTDA</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>João Pessoa</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>não cadastrado</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01765332000120</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>4731-8/00</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>Comércio varejista de combustíveis para veículos automotores</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:39:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>01.765.349/0001-87</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>TRANSPORTES ESCOLARES S.G. LTDA</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>sula.galvao@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01765349000187</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>4924-8/00</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>Transporte escolar</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:39:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>01.765.514/0001-09</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>AUTO DERVAL LTDA</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Teófilo Otoni</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>siare@escritaonline.cnt.br</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01765514000109</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>4530-7/03</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>Comércio a varejo de peças e acessórios novos para veículos automotores</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:39:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>01.765.712/0001-64</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>POSTO ALTO BONITO LTDA</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Valente</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>totinhacontabilidade@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01765712000164</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>4732-6/00</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>Comércio varejista de lubrificantes</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:40:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>01.766.076/0001-95</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>POSTO NOVO HORIZONTE LTDA</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>ES</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Serra</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>gruposchueng@gmail.com</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01766076000195</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>4731-8/00</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>Comércio varejista de combustíveis para veículos automotores</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:40:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>01.766.275/0001-01</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>R. M. KOTTWITZ MATERIAIS DE CONSTRUCAO LTDA</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Candelária</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>não cadastrado</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01766275000101</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>4744-0/99</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>Comércio varejista de materiais de construção em geral</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:40:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>01.766.605/0001-50</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>WSP BRASIL CONSULTORIA LTDA.</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>RJ</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>lcfdespachante@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01766605000150</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>7112-0/00</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>Serviços de engenharia</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:41:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>01.766.616/0001-30</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>AUTO POSTO ANHAIA MELLO LTDA</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>não cadastrado</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01766616000130</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>4731-8/00</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>Comércio varejista de combustíveis para veículos automotores</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:41:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>01.766.744/0001-84</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>RBC REDE BRASILEIRA DE COMUNICACAO S/A</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Divinópolis</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>fiscalmasterdivinopolis@gmail.com</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01766744000184</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>6022-5/02</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>Atividades relacionadas à televisão por assinatura, exceto programadoras</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:42:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>01.767.082/0001-67</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>EMPORIO LGB DISTRIBUIDORA DE PRODUTOS ALIMENTICIOS LTDA</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>São Carlos</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>emporiolgb@yahoo.com.br</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01767082000167</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>4711-3/02</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>Comércio varejista de mercadorias em geral, com predominância de produtos alimentícios - supermercados</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:42:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>01.767.097/0001-25</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>SANTOGAS COMERCIO DE GAS LTDA</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Cerqueira César</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>contato@vrcontabil.net</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01767097000125</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>4784-9/00</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>Comércio varejista de gás liqüefeito de petróleo (GLP)</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:42:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>01.767.692/0001-60</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>TRANSCONTINENTALLOG LOGISTICA E TRANSPORTES LTDA</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Uberlândia</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>diretoria@somaplace.com.br</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01767692000160</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>4930-2/02</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>Transporte rodoviário de carga, exceto produtos perigosos e mudanças, intermunicipal, interestadual e internacional</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:43:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>01.767.723/0001-83</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>PEWAG HELEVAR COMERCIO E IMPORTACAO DE PRODUTOS METALURGICOS LTDA</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Porto Alegre</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>luciane@helevar.com.br</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01767723000183</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>4685-1/00</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>Comércio atacadista de produtos siderúrgicos e metalúrgicos, exceto para construção</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:43:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>01.767.857/0001-02</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>SOCIEDADE EDUCACIONAL SARAH DAWSEY LTDA</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>RJ</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>não cadastrado</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01767857000102</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>8512-1/00</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>Educação infantil - pré-escola</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:44:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>01.767.883/0001-22</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>LABORATORIO QUIMIOAMBIENTAL LTDA</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Porto Alegre</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>qualidade@quimioambiental.com.br</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01767883000122</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>7120-1/00</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>Testes e análises técnicas</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:44:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>01.767.903/0001-65</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>CENTRALGAS - COMERCIO DE GAS E BEBIDAS LTDA</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Londrina</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>não cadastrado</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01767903000165</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>4784-9/00</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>Comércio varejista de gás liqüefeito de petróleo (GLP)</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:44:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>01.767.949/0001-84</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>DIAS &amp; SIQUEIRA COMERCIAL LTDA</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Aimorés</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>fiscal@contabilidadesantaluzia.com.br</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01767949000184</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>1011-2/01</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>Frigorífico - abate de bovinos</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:45:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>01.767.998/0001-17</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>VIACAO JAUA LTDA</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Salvador</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>ananeiva@viacaoregional.com.br</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01767998000117</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>4922-1/01</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>Transporte rodoviário coletivo de passageiros, com itinerário fixo, intermunicipal, exceto em região metropolitana</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:45:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>01.768.087/0001-04</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>LAZER TRANSPORTES LTDA</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Nova Odessa</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>contato@lazertransportes.com.br</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01768087000104</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>4924-8/00</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>Transporte escolar</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:46:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>01.768.089/0001-01</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>MERCADINHO F. C LTDA</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Salvador</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>tributario@bomfimnet.com</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01768089000101</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>4712-1/00</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>Comércio varejista de mercadorias em geral, com predominância de produtos alimentícios - minimercados, mercearias e armazéns</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:46:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>01.768.738/0001-66</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>PEREIRA GUEDES E GUEDES LTDA</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>Itumbiara</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>não cadastrado</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01768738000166</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>4731-8/00</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>Comércio varejista de combustíveis para veículos automotores</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:46:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>01.768.763/0001-40</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>BRASELIO INDUSTRIA E COMERCIO DE MAQUINAS LTDA</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Massaranduba</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>não cadastrado</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01768763000140</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>2833-0/00</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>Fabricação de máquinas e equipamentos para a agricultura e pecuária, peças e acessórios, exceto para irrigação</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:47:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>01.768.854/0001-85</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>AUTO POSTO AMBIENTAL LTDA</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Petrolina</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>jtorrescont@uol.com.br</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01768854000185</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>4731-8/00</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>Comércio varejista de combustíveis para veículos automotores</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:47:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>01.768.873/0001-01</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>AMCOM SISTEMAS DE INFORMACAO S/A</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Blumenau</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>não cadastrado</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01768873000101</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>6201-5/01</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>Desenvolvimento de programas de computador sob encomenda</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:48:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>01.769.155/0001-50</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>ANDREIA MIRIA SANTANA MATOS</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Tucano</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>farmaciaplantao13@gmail.com</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01769155000150</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>4771-7/01</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>Comércio varejista de produtos farmacêuticos, sem manipulação de fórmulas</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:48:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>01.769.350/0001-80</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>TRANSNI TRANSPORTES E TURISMO LTDA</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Vargem Grande Paulista</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>contato@transni.com.br</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01769350000180</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>4929-9/02</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>Transporte rodoviário coletivo de passageiros, sob regime de fretamento, intermunicipal, interestadual e internacional</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:48:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>01.769.569/0001-89</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>TV GUARARAPES S.A.</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Recife</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>financeiro@sistemaopiniao.com.br</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01769569000189</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>6021-7/00</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>Atividades de televisão aberta</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:49:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>01.769.792/0001-26</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>LATICINIO FERREIRA COSTA LTDA</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Itanhomi</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>ronaldoeroseli@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>https://cnpj.biz/01769792000126</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>1052-0/00</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>Fabricação de laticínios</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>2025-05-27 15:49:38</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>